<commit_message>
Fixed issue with column.AdjustToContents()
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -745,11 +745,10 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="9.270624999999999" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.410625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="9.700625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="12.700625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="15.550625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="7.1090625" style="0" customWidth="1"/>
+    <x:col min="3" max="4" width="9.1090625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="12.1090625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="17.1090625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>

<commit_message>
Fixed issue loading and saving sheets with different kinds of drawings.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -745,10 +745,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="7.1090625" style="0" customWidth="1"/>
-    <x:col min="3" max="4" width="9.1090625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="12.1090625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="17.1090625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="7.085625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="9.10125" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.085625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="12.10125" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="17.10125" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>

<commit_message>
Use System.Drawing.Graphics.MeasureString instead of System.Windows.Forms.TextRenderer for AdjustToContents.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -759,11 +759,11 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="9.270624999999999" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="10.410625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="9.700625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="12.700625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="15.550625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="7.980625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="9.000625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="8.580625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="11.950625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="15.590625000000001" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="1:6">

</xml_diff>

<commit_message>
Ensure all custom numbers formats start at 165 (0 - 164 are reserved). Don't output default number format (0, "").
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -67,8 +67,8 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="3">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="1" formatCode="$ #,##0"/>
-    <x:numFmt numFmtId="2" formatCode="MM/dd/yyyy"/>
+    <x:numFmt numFmtId="165" formatCode="$ #,##0"/>
+    <x:numFmt numFmtId="166" formatCode="MM/dd/yyyy"/>
   </x:numFmts>
   <x:fonts count="4">
     <x:font>
@@ -330,7 +330,7 @@
     <x:xf numFmtId="15" fontId="0" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -342,7 +342,7 @@
     <x:xf numFmtId="15" fontId="0" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -357,10 +357,10 @@
     <x:xf numFmtId="0" fontId="1" fillId="4" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -417,7 +417,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -433,7 +433,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -449,11 +449,11 @@
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>